<commit_message>
Started order analysis code; thread pooled the pdf to image conversion.
</commit_message>
<xml_diff>
--- a/PythonApplication1/archive_runs/ipr_read_data.xlsx
+++ b/PythonApplication1/archive_runs/ipr_read_data.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Johnny\Documents\UT_Law\2L Fall\Intellectual Property Tech Policy [Golden]\Final Paper\IPRAnalysis\IPRAnalysis\PythonApplication1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1659,8 +1664,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1728,6 +1733,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1774,7 +1787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1806,9 +1819,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1840,6 +1871,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2015,24 +2064,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="10" width="40.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="10" width="40.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2108,7 +2157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2146,7 +2195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -2184,7 +2233,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -2222,7 +2271,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -2260,7 +2309,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -2298,7 +2347,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -2336,7 +2385,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -2374,7 +2423,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>68</v>
       </c>
@@ -2412,7 +2461,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>74</v>
       </c>
@@ -2450,7 +2499,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>80</v>
       </c>
@@ -2488,7 +2537,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>86</v>
       </c>
@@ -2526,7 +2575,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>93</v>
       </c>
@@ -2564,7 +2613,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
@@ -2602,7 +2651,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>106</v>
       </c>
@@ -2640,7 +2689,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>112</v>
       </c>
@@ -2678,7 +2727,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>118</v>
       </c>
@@ -2716,7 +2765,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>125</v>
       </c>
@@ -2754,7 +2803,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>132</v>
       </c>
@@ -2792,7 +2841,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>138</v>
       </c>
@@ -2830,7 +2879,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>145</v>
       </c>
@@ -2868,7 +2917,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>149</v>
       </c>
@@ -2906,7 +2955,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>155</v>
       </c>
@@ -2944,7 +2993,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>158</v>
       </c>
@@ -2982,7 +3031,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>164</v>
       </c>
@@ -3020,7 +3069,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>172</v>
       </c>
@@ -3058,7 +3107,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>177</v>
       </c>
@@ -3096,7 +3145,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>181</v>
       </c>
@@ -3134,7 +3183,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>186</v>
       </c>
@@ -3172,7 +3221,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>191</v>
       </c>
@@ -3210,7 +3259,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>86</v>
       </c>
@@ -3248,7 +3297,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>195</v>
       </c>
@@ -3286,7 +3335,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>99</v>
       </c>
@@ -3324,7 +3373,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>201</v>
       </c>
@@ -3362,7 +3411,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>204</v>
       </c>
@@ -3400,7 +3449,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>211</v>
       </c>
@@ -3438,7 +3487,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>218</v>
       </c>
@@ -3476,7 +3525,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>221</v>
       </c>
@@ -3514,7 +3563,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>227</v>
       </c>
@@ -3552,7 +3601,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>232</v>
       </c>
@@ -3590,7 +3639,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>239</v>
       </c>
@@ -3628,7 +3677,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>242</v>
       </c>
@@ -3666,7 +3715,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>245</v>
       </c>
@@ -3704,7 +3753,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>248</v>
       </c>
@@ -3742,7 +3791,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>254</v>
       </c>
@@ -3780,7 +3829,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>259</v>
       </c>
@@ -3818,7 +3867,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>262</v>
       </c>
@@ -3856,7 +3905,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>267</v>
       </c>
@@ -3894,7 +3943,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>273</v>
       </c>
@@ -3932,7 +3981,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>278</v>
       </c>
@@ -3970,7 +4019,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>86</v>
       </c>
@@ -4008,7 +4057,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>195</v>
       </c>
@@ -4046,7 +4095,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>285</v>
       </c>
@@ -4084,7 +4133,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>291</v>
       </c>
@@ -4122,7 +4171,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>298</v>
       </c>
@@ -4160,7 +4209,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>304</v>
       </c>
@@ -4198,7 +4247,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>307</v>
       </c>
@@ -4236,7 +4285,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>313</v>
       </c>
@@ -4274,7 +4323,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>316</v>
       </c>
@@ -4312,7 +4361,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>322</v>
       </c>
@@ -4350,7 +4399,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>329</v>
       </c>
@@ -4388,7 +4437,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>335</v>
       </c>
@@ -4426,7 +4475,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>245</v>
       </c>
@@ -4464,7 +4513,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>339</v>
       </c>
@@ -4502,7 +4551,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>343</v>
       </c>
@@ -4540,7 +4589,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>347</v>
       </c>
@@ -4578,7 +4627,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>352</v>
       </c>
@@ -4616,7 +4665,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>356</v>
       </c>
@@ -4654,7 +4703,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>273</v>
       </c>
@@ -4686,7 +4735,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>278</v>
       </c>
@@ -4724,7 +4773,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>86</v>
       </c>
@@ -4762,7 +4811,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>364</v>
       </c>
@@ -4800,7 +4849,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>367</v>
       </c>
@@ -4838,7 +4887,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>372</v>
       </c>
@@ -4876,7 +4925,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" ht="69" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>375</v>
       </c>
@@ -4914,7 +4963,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>360</v>
       </c>
@@ -4943,7 +4992,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>382</v>
       </c>
@@ -4981,7 +5030,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>385</v>
       </c>
@@ -5019,7 +5068,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>391</v>
       </c>
@@ -5057,7 +5106,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>397</v>
       </c>
@@ -5095,7 +5144,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>400</v>
       </c>
@@ -5133,7 +5182,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>405</v>
       </c>
@@ -5171,7 +5220,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>411</v>
       </c>
@@ -5209,7 +5258,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>417</v>
       </c>
@@ -5247,7 +5296,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>420</v>
       </c>
@@ -5285,7 +5334,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>423</v>
       </c>
@@ -5323,7 +5372,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>245</v>
       </c>
@@ -5361,7 +5410,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>431</v>
       </c>
@@ -5399,7 +5448,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>434</v>
       </c>
@@ -5437,7 +5486,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>440</v>
       </c>
@@ -5475,7 +5524,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>445</v>
       </c>
@@ -5513,7 +5562,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>86</v>
       </c>
@@ -5551,7 +5600,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>448</v>
       </c>
@@ -5589,7 +5638,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>454</v>
       </c>
@@ -5627,7 +5676,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>372</v>
       </c>
@@ -5665,7 +5714,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>360</v>
       </c>
@@ -5694,7 +5743,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>461</v>
       </c>
@@ -5732,7 +5781,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>467</v>
       </c>
@@ -5770,7 +5819,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>471</v>
       </c>
@@ -5808,7 +5857,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>474</v>
       </c>
@@ -5846,7 +5895,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>480</v>
       </c>
@@ -5884,7 +5933,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>483</v>
       </c>
@@ -5922,7 +5971,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>485</v>
       </c>
@@ -5960,7 +6009,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>420</v>
       </c>
@@ -5998,7 +6047,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>489</v>
       </c>
@@ -6036,7 +6085,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>494</v>
       </c>
@@ -6074,7 +6123,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>500</v>
       </c>
@@ -6112,7 +6161,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>506</v>
       </c>
@@ -6150,7 +6199,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
update to claim analysis; added PatentsView API download
</commit_message>
<xml_diff>
--- a/PythonApplication1/archive_runs/ipr_read_data.xlsx
+++ b/PythonApplication1/archive_runs/ipr_read_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Johnny\Documents\UT_Law\2L Fall\Intellectual Property Tech Policy [Golden]\Final Paper\IPRAnalysis\IPRAnalysis\PythonApplication1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Johnny\Documents\UT_Law\2L Fall\Intellectual Property Tech Policy [Golden]\Final Paper\IPRAnalysis\IPRAnalysis\PythonApplication1\archive_runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="517">
   <si>
     <t>Trial Number(s)</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>IPR2014-01236</t>
-  </si>
-  <si>
-    <t>anuary29,2016</t>
   </si>
   <si>
     <t>FINAL WRITTEN DECISION Inter Partes Review</t>
@@ -229,9 +226,6 @@
   </si>
   <si>
     <t>IPR2014-01528</t>
-  </si>
-  <si>
-    <t>Mar.23,2015</t>
   </si>
   <si>
     <t>7783252</t>
@@ -853,9 +847,6 @@
 IPR2015-00822</t>
   </si>
   <si>
-    <t>anuary28,2016</t>
-  </si>
-  <si>
     <t>6425035</t>
   </si>
   <si>
@@ -1420,9 +1411,6 @@
     <t>IPR2014-01195</t>
   </si>
   <si>
-    <t>an.29,2016</t>
-  </si>
-  <si>
     <t>7787431</t>
   </si>
   <si>
@@ -1659,6 +1647,12 @@
   </si>
   <si>
     <t>0069-PGR2015-00005 final FD.pdf</t>
+  </si>
+  <si>
+    <t>01/28/2016</t>
+  </si>
+  <si>
+    <t>03/23/2015</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1725,6 +1719,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2067,7 +2064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2392,17 +2391,17 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>18</v>
@@ -2411,36 +2410,36 @@
         <v>19</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
@@ -2449,36 +2448,36 @@
         <v>19</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>39</v>
@@ -2487,36 +2486,36 @@
         <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>18</v>
@@ -2525,74 +2524,74 @@
         <v>19</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="K13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>18</v>
@@ -2601,74 +2600,74 @@
         <v>19</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="K15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>18</v>
@@ -2677,24 +2676,24 @@
         <v>19</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>30</v>
@@ -2706,7 +2705,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>18</v>
@@ -2715,36 +2714,36 @@
         <v>19</v>
       </c>
       <c r="I17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>39</v>
@@ -2753,36 +2752,36 @@
         <v>19</v>
       </c>
       <c r="I18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>39</v>
@@ -2791,36 +2790,36 @@
         <v>19</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>18</v>
@@ -2829,36 +2828,36 @@
         <v>19</v>
       </c>
       <c r="I20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>39</v>
@@ -2867,21 +2866,21 @@
         <v>19</v>
       </c>
       <c r="I21" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -2896,7 +2895,7 @@
         <v>16</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>18</v>
@@ -2908,18 +2907,18 @@
         <v>40</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
@@ -2931,10 +2930,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>39</v>
@@ -2943,21 +2942,21 @@
         <v>19</v>
       </c>
       <c r="I23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
@@ -2972,7 +2971,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>32</v>
@@ -2990,27 +2989,27 @@
         <v>19</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>32</v>
@@ -3019,59 +3018,59 @@
         <v>19</v>
       </c>
       <c r="I25" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="H26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="J26" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="3" t="s">
+      <c r="K26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>13</v>
@@ -3086,7 +3085,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>18</v>
@@ -3095,36 +3094,36 @@
         <v>19</v>
       </c>
       <c r="I27" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>39</v>
@@ -3133,27 +3132,27 @@
         <v>19</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>62</v>
+      <c r="C29" s="4" t="s">
+        <v>350</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
@@ -3162,7 +3161,7 @@
         <v>16</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>18</v>
@@ -3171,27 +3170,27 @@
         <v>19</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
@@ -3200,7 +3199,7 @@
         <v>16</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>32</v>
@@ -3209,27 +3208,27 @@
         <v>19</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>15</v>
@@ -3238,7 +3237,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>18</v>
@@ -3247,74 +3246,74 @@
         <v>19</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="J32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="K32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>18</v>
@@ -3323,65 +3322,65 @@
         <v>19</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="H34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="J34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="K34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>15</v>
@@ -3390,7 +3389,7 @@
         <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>32</v>
@@ -3399,36 +3398,36 @@
         <v>19</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>18</v>
@@ -3437,36 +3436,36 @@
         <v>19</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>39</v>
@@ -3475,36 +3474,36 @@
         <v>19</v>
       </c>
       <c r="I37" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>39</v>
@@ -3513,36 +3512,36 @@
         <v>19</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>39</v>
@@ -3551,21 +3550,21 @@
         <v>19</v>
       </c>
       <c r="I39" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>13</v>
@@ -3580,7 +3579,7 @@
         <v>16</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>39</v>
@@ -3589,36 +3588,36 @@
         <v>19</v>
       </c>
       <c r="I40" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>18</v>
@@ -3627,27 +3626,27 @@
         <v>19</v>
       </c>
       <c r="I41" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>15</v>
@@ -3656,7 +3655,7 @@
         <v>16</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>32</v>
@@ -3665,21 +3664,21 @@
         <v>19</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>13</v>
@@ -3703,7 +3702,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>34</v>
@@ -3712,12 +3711,12 @@
         <v>19</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>13</v>
@@ -3732,7 +3731,7 @@
         <v>16</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>18</v>
@@ -3744,33 +3743,33 @@
         <v>40</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>18</v>
@@ -3779,27 +3778,27 @@
         <v>19</v>
       </c>
       <c r="I45" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>15</v>
@@ -3808,7 +3807,7 @@
         <v>16</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>18</v>
@@ -3817,21 +3816,21 @@
         <v>19</v>
       </c>
       <c r="I46" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>13</v>
@@ -3846,7 +3845,7 @@
         <v>16</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>18</v>
@@ -3855,27 +3854,27 @@
         <v>19</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>263</v>
+      <c r="C48" s="4" t="s">
+        <v>515</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>15</v>
@@ -3884,7 +3883,7 @@
         <v>16</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>18</v>
@@ -3893,27 +3892,27 @@
         <v>19</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>15</v>
@@ -3922,7 +3921,7 @@
         <v>16</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>18</v>
@@ -3931,65 +3930,65 @@
         <v>19</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="J50" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="2" t="s">
+      <c r="K50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>15</v>
@@ -3998,7 +3997,7 @@
         <v>16</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>18</v>
@@ -4007,74 +4006,74 @@
         <v>19</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="H52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="J52" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="K52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>18</v>
@@ -4083,27 +4082,27 @@
         <v>19</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>15</v>
@@ -4112,7 +4111,7 @@
         <v>16</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>18</v>
@@ -4121,36 +4120,36 @@
         <v>19</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>39</v>
@@ -4159,27 +4158,27 @@
         <v>19</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>15</v>
@@ -4188,7 +4187,7 @@
         <v>16</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>18</v>
@@ -4197,36 +4196,36 @@
         <v>19</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>39</v>
@@ -4235,27 +4234,27 @@
         <v>19</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>15</v>
@@ -4264,7 +4263,7 @@
         <v>16</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>18</v>
@@ -4273,36 +4272,36 @@
         <v>19</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>32</v>
@@ -4311,27 +4310,27 @@
         <v>19</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>15</v>
@@ -4340,7 +4339,7 @@
         <v>16</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>18</v>
@@ -4349,74 +4348,74 @@
         <v>19</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="H61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I61" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="2" t="s">
+      <c r="J61" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="K61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L61" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>39</v>
@@ -4425,21 +4424,21 @@
         <v>19</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>13</v>
@@ -4454,7 +4453,7 @@
         <v>16</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>32</v>
@@ -4463,21 +4462,21 @@
         <v>19</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>13</v>
@@ -4492,7 +4491,7 @@
         <v>16</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>18</v>
@@ -4504,24 +4503,24 @@
         <v>40</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>15</v>
@@ -4530,7 +4529,7 @@
         <v>16</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>39</v>
@@ -4539,27 +4538,27 @@
         <v>19</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>15</v>
@@ -4568,7 +4567,7 @@
         <v>16</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>18</v>
@@ -4577,21 +4576,21 @@
         <v>19</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>13</v>
@@ -4606,7 +4605,7 @@
         <v>16</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>18</v>
@@ -4615,27 +4614,27 @@
         <v>19</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>15</v>
@@ -4644,7 +4643,7 @@
         <v>16</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>18</v>
@@ -4653,27 +4652,27 @@
         <v>19</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>15</v>
@@ -4682,7 +4681,7 @@
         <v>16</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>32</v>
@@ -4691,21 +4690,21 @@
         <v>19</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>13</v>
@@ -4714,36 +4713,36 @@
         <v>19</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>15</v>
@@ -4752,7 +4751,7 @@
         <v>16</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>18</v>
@@ -4761,74 +4760,74 @@
         <v>19</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="H72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="J72" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="K72" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>18</v>
@@ -4837,27 +4836,27 @@
         <v>19</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>15</v>
@@ -4866,7 +4865,7 @@
         <v>16</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>18</v>
@@ -4875,27 +4874,27 @@
         <v>19</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>15</v>
@@ -4904,7 +4903,7 @@
         <v>16</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>18</v>
@@ -4913,27 +4912,27 @@
         <v>19</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="69" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>15</v>
@@ -4942,7 +4941,7 @@
         <v>16</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>32</v>
@@ -4951,56 +4950,56 @@
         <v>19</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>15</v>
@@ -5009,36 +5008,36 @@
         <v>16</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>15</v>
@@ -5047,7 +5046,7 @@
         <v>16</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>18</v>
@@ -5056,27 +5055,27 @@
         <v>19</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>15</v>
@@ -5085,7 +5084,7 @@
         <v>16</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>18</v>
@@ -5094,36 +5093,36 @@
         <v>19</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>39</v>
@@ -5132,27 +5131,27 @@
         <v>19</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>15</v>
@@ -5161,7 +5160,7 @@
         <v>16</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>39</v>
@@ -5170,27 +5169,27 @@
         <v>19</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>15</v>
@@ -5199,7 +5198,7 @@
         <v>16</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>39</v>
@@ -5208,27 +5207,27 @@
         <v>19</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>15</v>
@@ -5237,7 +5236,7 @@
         <v>16</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>18</v>
@@ -5246,59 +5245,59 @@
         <v>19</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="J85" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K85" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>13</v>
@@ -5322,7 +5321,7 @@
         <v>19</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>34</v>
@@ -5331,27 +5330,27 @@
         <v>19</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>426</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>39</v>
@@ -5360,21 +5359,21 @@
         <v>19</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>13</v>
@@ -5389,7 +5388,7 @@
         <v>16</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>18</v>
@@ -5401,24 +5400,24 @@
         <v>40</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>15</v>
@@ -5427,7 +5426,7 @@
         <v>16</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>18</v>
@@ -5436,27 +5435,27 @@
         <v>19</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>15</v>
@@ -5465,7 +5464,7 @@
         <v>16</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>18</v>
@@ -5474,27 +5473,27 @@
         <v>19</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>441</v>
+      <c r="C91" s="4" t="s">
+        <v>350</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>15</v>
@@ -5503,7 +5502,7 @@
         <v>16</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>18</v>
@@ -5512,27 +5511,27 @@
         <v>19</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>15</v>
@@ -5541,74 +5540,74 @@
         <v>16</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C93" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F93" s="2" t="s">
+      <c r="H93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I93" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="J93" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H93" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I93" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="K93" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>15</v>
@@ -5617,7 +5616,7 @@
         <v>16</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>39</v>
@@ -5626,27 +5625,27 @@
         <v>19</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L94" s="3" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>15</v>
@@ -5655,7 +5654,7 @@
         <v>16</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>18</v>
@@ -5664,27 +5663,27 @@
         <v>19</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L95" s="3" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>15</v>
@@ -5693,7 +5692,7 @@
         <v>16</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>18</v>
@@ -5702,65 +5701,65 @@
         <v>19</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>18</v>
@@ -5769,27 +5768,27 @@
         <v>19</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="K98" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>15</v>
@@ -5798,7 +5797,7 @@
         <v>16</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>18</v>
@@ -5807,36 +5806,36 @@
         <v>19</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="K99" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>39</v>
@@ -5845,27 +5844,27 @@
         <v>19</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L100" s="3" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>15</v>
@@ -5874,7 +5873,7 @@
         <v>16</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>39</v>
@@ -5883,27 +5882,27 @@
         <v>19</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>15</v>
@@ -5912,7 +5911,7 @@
         <v>16</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>32</v>
@@ -5921,27 +5920,27 @@
         <v>19</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L102" s="3" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>15</v>
@@ -5950,7 +5949,7 @@
         <v>16</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>18</v>
@@ -5959,59 +5958,59 @@
         <v>19</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I104" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="J104" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L104" s="3" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>13</v>
@@ -6035,7 +6034,7 @@
         <v>19</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>34</v>
@@ -6044,12 +6043,12 @@
         <v>19</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>13</v>
@@ -6061,10 +6060,10 @@
         <v>15</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>32</v>
@@ -6073,36 +6072,36 @@
         <v>19</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="K106" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>18</v>
@@ -6111,65 +6110,65 @@
         <v>19</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="K107" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L107" s="3" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="J108" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F108" s="2" t="s">
+      <c r="K108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L108" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="J108" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L108" s="3" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>15</v>
@@ -6178,7 +6177,7 @@
         <v>16</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>18</v>
@@ -6187,27 +6186,27 @@
         <v>19</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="K109" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L109" s="3" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>15</v>
@@ -6216,7 +6215,7 @@
         <v>16</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>32</v>
@@ -6225,19 +6224,20 @@
         <v>19</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="K110" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>